<commit_message>
rearrange properties into separate folder
</commit_message>
<xml_diff>
--- a/spfx-locale.xlsx
+++ b/spfx-locale.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0B114F-277E-4B5E-BC96-88F490606E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10358D3-5FBF-4A3B-97A0-C9624D0B5D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="3405" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="146">
   <si>
     <t>key</t>
   </si>
@@ -432,12 +432,6 @@
   </si>
   <si>
     <t>UrlPickerBrowse</t>
-  </si>
-  <si>
-    <t>UrlPickerExtensions</t>
-  </si>
-  <si>
-    <t>.vsd\", \".vsdx\", \".vsdm</t>
   </si>
   <si>
     <t>View</t>
@@ -494,13 +488,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -514,14 +528,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E53">
-  <autoFilter ref="A1:E53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E52" dataDxfId="0">
+  <autoFilter ref="A1:E52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="en-us"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="de-de"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Translated"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WebPartStrings"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="en-us" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="de-de" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Translated" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WebPartStrings" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -849,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -881,887 +895,870 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D40" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D43" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D47" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C48" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="C48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C49" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="C49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D50" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C51" t="s">
-        <v>140</v>
-      </c>
-      <c r="D51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B52" t="s">
-        <v>141</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B52" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>143</v>
-      </c>
-      <c r="B53" t="s">
-        <v>144</v>
-      </c>
-      <c r="C53" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="C52" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>